<commit_message>
Template ROB Heading to Pascal
</commit_message>
<xml_diff>
--- a/template/Report ingestion Template v.1.0.xlsx
+++ b/template/Report ingestion Template v.1.0.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arjun S\source\repos\JsonConvert\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMM-LP-128\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9992D77C-7062-43F5-A0F9-9BA9434A4151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108D47BE-C155-4E2E-A759-CF36324B3E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,51 +43,6 @@
     <t>robs</t>
   </si>
   <si>
-    <t>remaining</t>
-  </si>
-  <si>
-    <t>propulsion</t>
-  </si>
-  <si>
-    <t>maneuver</t>
-  </si>
-  <si>
-    <t>generator</t>
-  </si>
-  <si>
-    <t>boiler</t>
-  </si>
-  <si>
-    <t>loaddischarge</t>
-  </si>
-  <si>
-    <t>deballast</t>
-  </si>
-  <si>
-    <t>igs</t>
-  </si>
-  <si>
-    <t>cargoheating</t>
-  </si>
-  <si>
-    <t>tankCleaning</t>
-  </si>
-  <si>
-    <t>incinerator</t>
-  </si>
-  <si>
-    <t>others</t>
-  </si>
-  <si>
-    <t>mainEngineConsumption</t>
-  </si>
-  <si>
-    <t>auxEngineConsumption</t>
-  </si>
-  <si>
-    <t>consumption</t>
-  </si>
-  <si>
     <t>MGO</t>
   </si>
   <si>
@@ -202,12 +169,6 @@
     <t>remarks2</t>
   </si>
   <si>
-    <t>tankcleaning</t>
-  </si>
-  <si>
-    <t>cooling</t>
-  </si>
-  <si>
     <t>EventType</t>
   </si>
   <si>
@@ -248,6 +209,57 @@
   </si>
   <si>
     <t>0.000</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Propulsion</t>
+  </si>
+  <si>
+    <t>Maneuver</t>
+  </si>
+  <si>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>Boiler</t>
+  </si>
+  <si>
+    <t>DeBallast</t>
+  </si>
+  <si>
+    <t>Igs</t>
+  </si>
+  <si>
+    <t>CargoHeating</t>
+  </si>
+  <si>
+    <t>TankCleaning</t>
+  </si>
+  <si>
+    <t>Deballast</t>
+  </si>
+  <si>
+    <t>Incinerator</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>MainEngineConsumption</t>
+  </si>
+  <si>
+    <t>AuxEngineConsumption</t>
+  </si>
+  <si>
+    <t>Consumption</t>
+  </si>
+  <si>
+    <t>LoadDischarge</t>
+  </si>
+  <si>
+    <t>Cooling</t>
   </si>
 </sst>
 </file>
@@ -628,80 +640,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1656C47-B37D-4BA1-9070-1AAF9363FE26}">
   <dimension ref="A1:FB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DC1" workbookViewId="0">
-      <selection activeCell="DT3" sqref="DT3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="35.5546875" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
-    <col min="13" max="13" width="27.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="35.54296875" customWidth="1"/>
+    <col min="6" max="6" width="7.6328125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="8" max="9" width="11.36328125" customWidth="1"/>
+    <col min="10" max="10" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6328125" customWidth="1"/>
+    <col min="13" max="13" width="27.54296875" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="13.36328125" customWidth="1"/>
     <col min="17" max="17" width="21" customWidth="1"/>
-    <col min="18" max="18" width="5.88671875" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" customWidth="1"/>
-    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.33203125" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" customWidth="1"/>
-    <col min="25" max="25" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.44140625" customWidth="1"/>
+    <col min="18" max="18" width="5.90625" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" customWidth="1"/>
+    <col min="20" max="20" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.36328125" customWidth="1"/>
+    <col min="24" max="24" width="12.08984375" customWidth="1"/>
+    <col min="25" max="25" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.453125" customWidth="1"/>
     <col min="27" max="27" width="20" customWidth="1"/>
-    <col min="28" max="28" width="10.33203125" customWidth="1"/>
-    <col min="29" max="29" width="39.44140625" customWidth="1"/>
-    <col min="30" max="30" width="27.33203125" customWidth="1"/>
-    <col min="31" max="31" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.33203125" customWidth="1"/>
+    <col min="28" max="28" width="10.36328125" customWidth="1"/>
+    <col min="29" max="29" width="39.453125" customWidth="1"/>
+    <col min="30" max="30" width="27.36328125" customWidth="1"/>
+    <col min="31" max="31" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.36328125" customWidth="1"/>
     <col min="33" max="33" width="20" customWidth="1"/>
-    <col min="34" max="34" width="9.33203125" customWidth="1"/>
-    <col min="35" max="35" width="9.6640625" customWidth="1"/>
-    <col min="36" max="36" width="9.109375" customWidth="1"/>
+    <col min="34" max="34" width="9.36328125" customWidth="1"/>
+    <col min="35" max="35" width="9.6328125" customWidth="1"/>
+    <col min="36" max="36" width="9.08984375" customWidth="1"/>
     <col min="37" max="37" width="9" customWidth="1"/>
-    <col min="38" max="38" width="5.6640625" customWidth="1"/>
-    <col min="39" max="39" width="12.6640625" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" customWidth="1"/>
-    <col min="41" max="41" width="3.6640625" customWidth="1"/>
-    <col min="42" max="42" width="11.88671875" customWidth="1"/>
+    <col min="38" max="38" width="5.6328125" customWidth="1"/>
+    <col min="39" max="39" width="12.6328125" customWidth="1"/>
+    <col min="40" max="40" width="8.6328125" customWidth="1"/>
+    <col min="41" max="41" width="3.6328125" customWidth="1"/>
+    <col min="42" max="42" width="11.90625" customWidth="1"/>
     <col min="43" max="43" width="12" customWidth="1"/>
-    <col min="44" max="44" width="9.88671875" customWidth="1"/>
-    <col min="45" max="45" width="6.44140625" customWidth="1"/>
-    <col min="46" max="46" width="21.88671875" customWidth="1"/>
-    <col min="47" max="47" width="20.88671875" customWidth="1"/>
-    <col min="48" max="48" width="11.88671875" customWidth="1"/>
-    <col min="49" max="49" width="9.33203125" customWidth="1"/>
-    <col min="50" max="50" width="9.6640625" customWidth="1"/>
-    <col min="51" max="51" width="9.109375" customWidth="1"/>
+    <col min="44" max="44" width="9.90625" customWidth="1"/>
+    <col min="45" max="45" width="6.453125" customWidth="1"/>
+    <col min="46" max="46" width="21.90625" customWidth="1"/>
+    <col min="47" max="47" width="20.90625" customWidth="1"/>
+    <col min="48" max="48" width="11.90625" customWidth="1"/>
+    <col min="49" max="49" width="9.36328125" customWidth="1"/>
+    <col min="50" max="50" width="9.6328125" customWidth="1"/>
+    <col min="51" max="51" width="9.08984375" customWidth="1"/>
     <col min="52" max="52" width="9" customWidth="1"/>
-    <col min="53" max="53" width="5.6640625" customWidth="1"/>
-    <col min="54" max="54" width="12.6640625" customWidth="1"/>
-    <col min="55" max="55" width="8.6640625" customWidth="1"/>
-    <col min="56" max="56" width="3.6640625" customWidth="1"/>
-    <col min="57" max="57" width="11.88671875" customWidth="1"/>
+    <col min="53" max="53" width="5.6328125" customWidth="1"/>
+    <col min="54" max="54" width="12.6328125" customWidth="1"/>
+    <col min="55" max="55" width="8.6328125" customWidth="1"/>
+    <col min="56" max="56" width="3.6328125" customWidth="1"/>
+    <col min="57" max="57" width="11.90625" customWidth="1"/>
     <col min="58" max="58" width="12" customWidth="1"/>
-    <col min="59" max="59" width="9.88671875" customWidth="1"/>
-    <col min="60" max="60" width="6.44140625" customWidth="1"/>
-    <col min="61" max="61" width="21.88671875" customWidth="1"/>
-    <col min="62" max="62" width="20.88671875" customWidth="1"/>
-    <col min="63" max="63" width="11.88671875" customWidth="1"/>
-    <col min="123" max="123" width="11.77734375" customWidth="1"/>
-    <col min="124" max="124" width="10.44140625" customWidth="1"/>
+    <col min="59" max="59" width="9.90625" customWidth="1"/>
+    <col min="60" max="60" width="6.453125" customWidth="1"/>
+    <col min="61" max="61" width="21.90625" customWidth="1"/>
+    <col min="62" max="62" width="20.90625" customWidth="1"/>
+    <col min="63" max="63" width="11.90625" customWidth="1"/>
+    <col min="123" max="123" width="11.81640625" customWidth="1"/>
+    <col min="124" max="124" width="10.453125" customWidth="1"/>
     <col min="126" max="126" width="12" customWidth="1"/>
-    <col min="127" max="127" width="13.88671875" customWidth="1"/>
-    <col min="142" max="142" width="8.6640625" customWidth="1"/>
-    <col min="152" max="152" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="13.90625" customWidth="1"/>
+    <col min="142" max="142" width="8.6328125" customWidth="1"/>
+    <col min="152" max="152" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:158" x14ac:dyDescent="0.25">
@@ -800,16 +812,16 @@
     </row>
     <row r="2" spans="1:158" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>0</v>
@@ -818,88 +830,88 @@
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="AH2" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="AI2" s="4"/>
       <c r="AJ2" s="4"/>
@@ -916,7 +928,7 @@
       <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
       <c r="AW2" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AX2" s="4"/>
       <c r="AY2" s="4"/>
@@ -933,7 +945,7 @@
       <c r="BJ2" s="4"/>
       <c r="BK2" s="4"/>
       <c r="BL2" s="4" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="BM2" s="4"/>
       <c r="BN2" s="4"/>
@@ -950,7 +962,7 @@
       <c r="BY2" s="4"/>
       <c r="BZ2" s="4"/>
       <c r="CA2" s="4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="CB2" s="4"/>
       <c r="CC2" s="4"/>
@@ -967,7 +979,7 @@
       <c r="CN2" s="4"/>
       <c r="CO2" s="4"/>
       <c r="CP2" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="CQ2" s="4"/>
       <c r="CR2" s="4"/>
@@ -984,7 +996,7 @@
       <c r="DC2" s="4"/>
       <c r="DD2" s="4"/>
       <c r="DE2" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="DF2" s="4"/>
       <c r="DG2" s="4"/>
@@ -1006,7 +1018,7 @@
       <c r="DW2" s="1"/>
       <c r="DX2" s="1"/>
       <c r="DY2" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="DZ2" s="4"/>
       <c r="EA2" s="4"/>
@@ -1020,7 +1032,7 @@
       <c r="EI2" s="4"/>
       <c r="EJ2" s="4"/>
       <c r="EK2" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="EL2" s="4"/>
       <c r="EM2" s="4"/>
@@ -1040,7 +1052,7 @@
       <c r="FA2" s="2"/>
       <c r="FB2" s="2"/>
     </row>
-    <row r="3" spans="1:158" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:158" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1075,355 +1087,355 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
       <c r="AH3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="AI3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="AJ3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="AK3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="AL3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="AM3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="AN3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="AO3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="AP3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="AQ3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="AR3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="AS3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="AT3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="AU3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="AV3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="AW3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="AX3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="AY3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="AZ3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="BA3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="BB3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="BC3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="BD3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="BE3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="BF3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="BG3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="BH3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="BI3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="BJ3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="BK3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="BL3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="BM3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="BN3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="BO3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="BP3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="BQ3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="BR3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="BS3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="BT3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="BU3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="BV3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="BW3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="BX3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="BY3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="BZ3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="CA3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="CB3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="CC3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="CD3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="CE3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="CF3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="CG3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="CH3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="CI3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="CJ3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="CK3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="CL3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="CM3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="CN3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="CO3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="CP3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="CQ3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="CR3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="CS3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="CT3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="CU3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="CV3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="CW3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="CX3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="CY3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="CZ3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="DA3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="DB3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="DC3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="DE3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="DF3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="DG3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="DH3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="DI3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="DJ3" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="DK3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="DL3" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="DM3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="DN3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="DO3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="DP3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="DQ3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="DR3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="DT3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="DU3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="DV3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="DW3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="DX3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="DY3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="DZ3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="EA3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="EB3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="EC3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="ED3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="EE3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="EF3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="EG3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="DU3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="DV3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="DW3" s="3" t="s">
+      <c r="EH3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="EI3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="EJ3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="EK3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="EL3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="EM3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="EN3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="DX3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="DY3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="DZ3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="EA3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="EB3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="EC3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="ED3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="EE3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="EF3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="EG3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="EH3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="EI3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="EJ3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="EK3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="EL3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="EM3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="EN3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="EO3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="EP3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="EQ3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="ER3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="ES3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="ET3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="EU3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="EV3" s="3" t="s">
-        <v>17</v>
+      <c r="EO3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="EP3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="EQ3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="ER3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="ES3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="ET3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="EU3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="EV3" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:158" x14ac:dyDescent="0.25">
@@ -1797,180 +1809,180 @@
         <v>123</v>
       </c>
       <c r="DT4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="DU4">
         <v>44</v>
       </c>
       <c r="DV4" t="s">
+        <v>40</v>
+      </c>
+      <c r="DW4" t="s">
+        <v>41</v>
+      </c>
+      <c r="DX4" t="s">
+        <v>42</v>
+      </c>
+      <c r="DY4" t="s">
+        <v>50</v>
+      </c>
+      <c r="DZ4" t="s">
+        <v>51</v>
+      </c>
+      <c r="EA4" t="s">
+        <v>51</v>
+      </c>
+      <c r="EB4" t="s">
+        <v>51</v>
+      </c>
+      <c r="EC4" t="s">
+        <v>51</v>
+      </c>
+      <c r="ED4" t="s">
+        <v>51</v>
+      </c>
+      <c r="EE4" t="s">
+        <v>51</v>
+      </c>
+      <c r="EF4" t="s">
+        <v>51</v>
+      </c>
+      <c r="EG4" t="s">
+        <v>52</v>
+      </c>
+      <c r="EH4" t="s">
+        <v>53</v>
+      </c>
+      <c r="EI4" t="s">
+        <v>54</v>
+      </c>
+      <c r="EJ4" t="s">
         <v>55</v>
       </c>
-      <c r="DW4" t="s">
-        <v>56</v>
-      </c>
-      <c r="DX4" t="s">
-        <v>57</v>
-      </c>
-      <c r="DY4" t="s">
-        <v>67</v>
-      </c>
-      <c r="DZ4" t="s">
-        <v>68</v>
-      </c>
-      <c r="EA4" t="s">
-        <v>68</v>
-      </c>
-      <c r="EB4" t="s">
-        <v>68</v>
-      </c>
-      <c r="EC4" t="s">
-        <v>68</v>
-      </c>
-      <c r="ED4" t="s">
-        <v>68</v>
-      </c>
-      <c r="EE4" t="s">
-        <v>68</v>
-      </c>
-      <c r="EF4" t="s">
-        <v>68</v>
-      </c>
-      <c r="EG4" t="s">
-        <v>69</v>
-      </c>
-      <c r="EH4" t="s">
-        <v>70</v>
-      </c>
-      <c r="EI4" t="s">
-        <v>71</v>
-      </c>
-      <c r="EJ4" t="s">
-        <v>72</v>
-      </c>
       <c r="EK4" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="EL4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EM4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EN4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EO4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EP4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EQ4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="ER4" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="ES4" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="ET4" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="EU4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="EV4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:158" x14ac:dyDescent="0.25">
       <c r="DT5" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="DU5">
         <v>44</v>
       </c>
       <c r="DV5" t="s">
+        <v>40</v>
+      </c>
+      <c r="DW5" t="s">
+        <v>41</v>
+      </c>
+      <c r="DX5" t="s">
+        <v>44</v>
+      </c>
+      <c r="DY5" t="s">
+        <v>56</v>
+      </c>
+      <c r="DZ5" t="s">
+        <v>57</v>
+      </c>
+      <c r="EA5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EB5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EC5" t="s">
+        <v>51</v>
+      </c>
+      <c r="ED5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EE5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EF5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EG5" t="s">
+        <v>51</v>
+      </c>
+      <c r="EH5" t="s">
+        <v>52</v>
+      </c>
+      <c r="EI5" t="s">
+        <v>53</v>
+      </c>
+      <c r="EJ5" t="s">
+        <v>54</v>
+      </c>
+      <c r="EK5" t="s">
         <v>55</v>
       </c>
-      <c r="DW5" t="s">
+      <c r="EL5" t="s">
+        <v>58</v>
+      </c>
+      <c r="EM5" t="s">
         <v>56</v>
       </c>
-      <c r="DX5" t="s">
-        <v>59</v>
-      </c>
-      <c r="DY5" t="s">
-        <v>73</v>
-      </c>
-      <c r="DZ5" t="s">
-        <v>74</v>
-      </c>
-      <c r="EA5" t="s">
-        <v>68</v>
-      </c>
-      <c r="EB5" t="s">
-        <v>68</v>
-      </c>
-      <c r="EC5" t="s">
-        <v>68</v>
-      </c>
-      <c r="ED5" t="s">
-        <v>68</v>
-      </c>
-      <c r="EE5" t="s">
-        <v>68</v>
-      </c>
-      <c r="EF5" t="s">
-        <v>68</v>
-      </c>
-      <c r="EG5" t="s">
-        <v>68</v>
-      </c>
-      <c r="EH5" t="s">
-        <v>69</v>
-      </c>
-      <c r="EI5" t="s">
-        <v>70</v>
-      </c>
-      <c r="EJ5" t="s">
-        <v>71</v>
-      </c>
-      <c r="EK5" t="s">
-        <v>72</v>
-      </c>
-      <c r="EL5" t="s">
-        <v>75</v>
-      </c>
-      <c r="EM5" t="s">
-        <v>73</v>
-      </c>
       <c r="EN5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="EO5" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EP5" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EQ5" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="ER5" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="ES5" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="ET5" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EU5" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="EV5" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:158" x14ac:dyDescent="0.25">
@@ -2390,5 +2402,6 @@
     <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>